<commit_message>
Auto commit at 2025-08-30 17:03:57.19
</commit_message>
<xml_diff>
--- a/data/cddata.xlsx
+++ b/data/cddata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="81">
   <si>
     <t>11150kw</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -159,44 +159,14 @@
     <t>2018年</t>
   </si>
   <si>
-    <t>626,624.99 kWh</t>
-  </si>
-  <si>
     <t>2019年</t>
   </si>
   <si>
-    <t>2,487,651.48 kWh</t>
-  </si>
-  <si>
-    <t>3,580,420.55 kWh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2021年</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>2020年</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4,883,217.96 kWh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5,136,589.43 kWh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5,076,097.29 kWh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6,674,722.09 kWh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3,395,628.58 kWh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -371,7 +341,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;¥&quot;#,##0.00;[Red]&quot;¥&quot;\-#,##0.00"/>
+    <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -412,8 +382,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -739,15 +709,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" t="s">
         <v>77</v>
-      </c>
-      <c r="B2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -755,7 +725,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -763,15 +733,15 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -779,7 +749,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -787,7 +757,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -795,7 +765,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
@@ -803,10 +773,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -930,7 +900,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -938,7 +908,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -946,7 +916,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -954,7 +924,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>14</v>
@@ -962,7 +932,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -998,7 +968,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
@@ -1006,7 +976,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
@@ -1014,7 +984,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -1022,7 +992,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
@@ -1057,7 +1027,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
@@ -1065,7 +1035,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
         <v>21</v>
@@ -1073,7 +1043,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
@@ -1081,7 +1051,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
@@ -1097,7 +1067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1120,7 +1090,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
@@ -1131,7 +1101,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
         <v>29</v>
@@ -1142,7 +1112,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
         <v>31</v>
@@ -1159,10 +1129,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1186,89 +1156,92 @@
       <c r="A2" t="s">
         <v>35</v>
       </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2" s="1">
+        <v>626624.99</v>
+      </c>
+      <c r="C2" s="3">
         <v>419522.88</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="2">
+        <v>36</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2487651.48</v>
+      </c>
+      <c r="C3" s="3">
         <v>1298604.49</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="2">
+        <v>38</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3580420.55</v>
+      </c>
+      <c r="C4" s="3">
         <v>1340324.3400000001</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="2">
+        <v>37</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4883217.96</v>
+      </c>
+      <c r="C5" s="3">
         <v>1541061.48</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="2">
+        <v>39</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5136589.43</v>
+      </c>
+      <c r="C6" s="3">
         <v>2141138.69</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="2">
+        <v>40</v>
+      </c>
+      <c r="B7" s="1">
+        <v>5076097.29</v>
+      </c>
+      <c r="C7" s="3">
         <v>1765909.85</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="2">
+        <v>41</v>
+      </c>
+      <c r="B8" s="1">
+        <v>6674722.0899999999</v>
+      </c>
+      <c r="C8" s="3">
         <v>1775147.16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="2">
+        <v>42</v>
+      </c>
+      <c r="B9" s="1">
+        <v>3395628.58</v>
+      </c>
+      <c r="C9" s="3">
         <v>963642.56</v>
       </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C10" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1293,21 +1266,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B2">
         <v>29833145.190000001</v>
@@ -1321,7 +1294,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B3">
         <v>2027807.18</v>
@@ -1356,10 +1329,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
         <v>34</v>
@@ -1367,9 +1340,9 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="3">
+        <v>54</v>
+      </c>
+      <c r="B2" s="2">
         <v>0</v>
       </c>
       <c r="C2">
@@ -1378,9 +1351,9 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" s="3">
+        <v>55</v>
+      </c>
+      <c r="B3" s="2">
         <v>0</v>
       </c>
       <c r="C3">
@@ -1389,9 +1362,9 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" s="3">
+        <v>54</v>
+      </c>
+      <c r="B4" s="2">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="C4">
@@ -1400,9 +1373,9 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" s="3">
+        <v>55</v>
+      </c>
+      <c r="B5" s="2">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="C5">
@@ -1411,9 +1384,9 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="3">
+        <v>54</v>
+      </c>
+      <c r="B6" s="2">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C6">
@@ -1422,9 +1395,9 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" s="3">
+        <v>55</v>
+      </c>
+      <c r="B7" s="2">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C7">
@@ -1433,9 +1406,9 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B8" s="3">
+        <v>54</v>
+      </c>
+      <c r="B8" s="2">
         <v>0.125</v>
       </c>
       <c r="C8">
@@ -1444,9 +1417,9 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B9" s="3">
+        <v>55</v>
+      </c>
+      <c r="B9" s="2">
         <v>0.125</v>
       </c>
       <c r="C9">
@@ -1455,9 +1428,9 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="3">
+        <v>54</v>
+      </c>
+      <c r="B10" s="2">
         <v>0.16666666666666666</v>
       </c>
       <c r="C10">
@@ -1466,9 +1439,9 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="3">
+        <v>55</v>
+      </c>
+      <c r="B11" s="2">
         <v>0.16666666666666666</v>
       </c>
       <c r="C11">
@@ -1477,9 +1450,9 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="3">
+        <v>54</v>
+      </c>
+      <c r="B12" s="2">
         <v>0.20833333333333334</v>
       </c>
       <c r="C12">
@@ -1488,9 +1461,9 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="3">
+        <v>55</v>
+      </c>
+      <c r="B13" s="2">
         <v>0.20833333333333334</v>
       </c>
       <c r="C13">
@@ -1499,9 +1472,9 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14" s="3">
+        <v>54</v>
+      </c>
+      <c r="B14" s="2">
         <v>0.25</v>
       </c>
       <c r="C14">
@@ -1510,9 +1483,9 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" s="3">
+        <v>55</v>
+      </c>
+      <c r="B15" s="2">
         <v>0.25</v>
       </c>
       <c r="C15">
@@ -1521,9 +1494,9 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="3">
+        <v>54</v>
+      </c>
+      <c r="B16" s="2">
         <v>0.29166666666666669</v>
       </c>
       <c r="C16">
@@ -1532,9 +1505,9 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" s="3">
+        <v>55</v>
+      </c>
+      <c r="B17" s="2">
         <v>0.29166666666666669</v>
       </c>
       <c r="C17">
@@ -1543,9 +1516,9 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18" s="3">
+        <v>54</v>
+      </c>
+      <c r="B18" s="2">
         <v>0.33333333333333331</v>
       </c>
       <c r="C18">
@@ -1554,9 +1527,9 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19" s="3">
+        <v>55</v>
+      </c>
+      <c r="B19" s="2">
         <v>0.33333333333333331</v>
       </c>
       <c r="C19">
@@ -1565,9 +1538,9 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" s="3">
+        <v>54</v>
+      </c>
+      <c r="B20" s="2">
         <v>0.375</v>
       </c>
       <c r="C20">
@@ -1576,9 +1549,9 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>63</v>
-      </c>
-      <c r="B21" s="3">
+        <v>55</v>
+      </c>
+      <c r="B21" s="2">
         <v>0.375</v>
       </c>
       <c r="C21">
@@ -1587,9 +1560,9 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>62</v>
-      </c>
-      <c r="B22" s="3">
+        <v>54</v>
+      </c>
+      <c r="B22" s="2">
         <v>0.41666666666666669</v>
       </c>
       <c r="C22">
@@ -1598,9 +1571,9 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>63</v>
-      </c>
-      <c r="B23" s="3">
+        <v>55</v>
+      </c>
+      <c r="B23" s="2">
         <v>0.41666666666666669</v>
       </c>
       <c r="C23">
@@ -1609,9 +1582,9 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" s="3">
+        <v>54</v>
+      </c>
+      <c r="B24" s="2">
         <v>0.45833333333333331</v>
       </c>
       <c r="C24">
@@ -1620,9 +1593,9 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>63</v>
-      </c>
-      <c r="B25" s="3">
+        <v>55</v>
+      </c>
+      <c r="B25" s="2">
         <v>0.45833333333333331</v>
       </c>
       <c r="C25">
@@ -1631,9 +1604,9 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>62</v>
-      </c>
-      <c r="B26" s="3">
+        <v>54</v>
+      </c>
+      <c r="B26" s="2">
         <v>0.5</v>
       </c>
       <c r="C26">
@@ -1642,9 +1615,9 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" s="3">
+        <v>55</v>
+      </c>
+      <c r="B27" s="2">
         <v>0.5</v>
       </c>
       <c r="C27">
@@ -1653,9 +1626,9 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>62</v>
-      </c>
-      <c r="B28" s="3">
+        <v>54</v>
+      </c>
+      <c r="B28" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="C28">
@@ -1664,9 +1637,9 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>63</v>
-      </c>
-      <c r="B29" s="3">
+        <v>55</v>
+      </c>
+      <c r="B29" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="C29">
@@ -1675,9 +1648,9 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>62</v>
-      </c>
-      <c r="B30" s="3">
+        <v>54</v>
+      </c>
+      <c r="B30" s="2">
         <v>0.58333333333333337</v>
       </c>
       <c r="C30">
@@ -1686,9 +1659,9 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>63</v>
-      </c>
-      <c r="B31" s="3">
+        <v>55</v>
+      </c>
+      <c r="B31" s="2">
         <v>0.58333333333333337</v>
       </c>
       <c r="C31">
@@ -1697,9 +1670,9 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" s="3">
+        <v>54</v>
+      </c>
+      <c r="B32" s="2">
         <v>0.625</v>
       </c>
       <c r="C32">
@@ -1708,9 +1681,9 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="3">
+        <v>55</v>
+      </c>
+      <c r="B33" s="2">
         <v>0.625</v>
       </c>
       <c r="C33">
@@ -1719,9 +1692,9 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>62</v>
-      </c>
-      <c r="B34" s="3">
+        <v>54</v>
+      </c>
+      <c r="B34" s="2">
         <v>0.66666666666666663</v>
       </c>
       <c r="C34">
@@ -1730,9 +1703,9 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>63</v>
-      </c>
-      <c r="B35" s="3">
+        <v>55</v>
+      </c>
+      <c r="B35" s="2">
         <v>0.66666666666666663</v>
       </c>
       <c r="C35">
@@ -1741,9 +1714,9 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>62</v>
-      </c>
-      <c r="B36" s="3">
+        <v>54</v>
+      </c>
+      <c r="B36" s="2">
         <v>0.70833333333333337</v>
       </c>
       <c r="C36">
@@ -1752,9 +1725,9 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>63</v>
-      </c>
-      <c r="B37" s="3">
+        <v>55</v>
+      </c>
+      <c r="B37" s="2">
         <v>0.70833333333333337</v>
       </c>
       <c r="C37">
@@ -1763,9 +1736,9 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>62</v>
-      </c>
-      <c r="B38" s="3">
+        <v>54</v>
+      </c>
+      <c r="B38" s="2">
         <v>0.75</v>
       </c>
       <c r="C38">
@@ -1774,9 +1747,9 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>63</v>
-      </c>
-      <c r="B39" s="3">
+        <v>55</v>
+      </c>
+      <c r="B39" s="2">
         <v>0.75</v>
       </c>
       <c r="C39">
@@ -1785,9 +1758,9 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>62</v>
-      </c>
-      <c r="B40" s="3">
+        <v>54</v>
+      </c>
+      <c r="B40" s="2">
         <v>0.79166666666666663</v>
       </c>
       <c r="C40">
@@ -1796,9 +1769,9 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>63</v>
-      </c>
-      <c r="B41" s="3">
+        <v>55</v>
+      </c>
+      <c r="B41" s="2">
         <v>0.79166666666666663</v>
       </c>
       <c r="C41">
@@ -1807,9 +1780,9 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>62</v>
-      </c>
-      <c r="B42" s="3">
+        <v>54</v>
+      </c>
+      <c r="B42" s="2">
         <v>0.83333333333333337</v>
       </c>
       <c r="C42">
@@ -1818,9 +1791,9 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>63</v>
-      </c>
-      <c r="B43" s="3">
+        <v>55</v>
+      </c>
+      <c r="B43" s="2">
         <v>0.83333333333333337</v>
       </c>
       <c r="C43">
@@ -1829,9 +1802,9 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>62</v>
-      </c>
-      <c r="B44" s="3">
+        <v>54</v>
+      </c>
+      <c r="B44" s="2">
         <v>0.875</v>
       </c>
       <c r="C44">
@@ -1840,9 +1813,9 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>63</v>
-      </c>
-      <c r="B45" s="3">
+        <v>55</v>
+      </c>
+      <c r="B45" s="2">
         <v>0.875</v>
       </c>
       <c r="C45">
@@ -1851,9 +1824,9 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>62</v>
-      </c>
-      <c r="B46" s="3">
+        <v>54</v>
+      </c>
+      <c r="B46" s="2">
         <v>0.91666666666666663</v>
       </c>
       <c r="C46">
@@ -1862,9 +1835,9 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>63</v>
-      </c>
-      <c r="B47" s="3">
+        <v>55</v>
+      </c>
+      <c r="B47" s="2">
         <v>0.91666666666666663</v>
       </c>
       <c r="C47">
@@ -1873,9 +1846,9 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>62</v>
-      </c>
-      <c r="B48" s="3">
+        <v>54</v>
+      </c>
+      <c r="B48" s="2">
         <v>0.95833333333333337</v>
       </c>
       <c r="C48">
@@ -1884,9 +1857,9 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>63</v>
-      </c>
-      <c r="B49" s="3">
+        <v>55</v>
+      </c>
+      <c r="B49" s="2">
         <v>0.95833333333333337</v>
       </c>
       <c r="C49">
@@ -1916,21 +1889,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B2">
         <v>28527002.210000001</v>
@@ -1944,7 +1917,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B3">
         <v>1626933.96</v>

</xml_diff>

<commit_message>
Auto commit at 2025-08-30 17:23:06.97
</commit_message>
<xml_diff>
--- a/data/cddata.xlsx
+++ b/data/cddata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="89">
   <si>
     <t>11150kw</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -159,14 +159,44 @@
     <t>2018年</t>
   </si>
   <si>
+    <t>626,624.99 kWh</t>
+  </si>
+  <si>
     <t>2019年</t>
   </si>
   <si>
+    <t>2,487,651.48 kWh</t>
+  </si>
+  <si>
+    <t>3,580,420.55 kWh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>2021年</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>2020年</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4,883,217.96 kWh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5,136,589.43 kWh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5,076,097.29 kWh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6,674,722.09 kWh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3,395,628.58 kWh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -341,7 +371,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;¥&quot;#,##0.00;[Red]&quot;¥&quot;\-#,##0.00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -382,8 +412,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -709,15 +739,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -725,7 +755,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -733,15 +763,15 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -749,7 +779,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -757,7 +787,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -765,7 +795,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
@@ -773,10 +803,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -900,7 +930,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -908,7 +938,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -916,7 +946,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -924,7 +954,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>14</v>
@@ -932,7 +962,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -968,7 +998,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
@@ -976,7 +1006,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
@@ -984,7 +1014,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -992,7 +1022,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
@@ -1027,7 +1057,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
@@ -1035,7 +1065,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
         <v>21</v>
@@ -1043,7 +1073,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
@@ -1051,7 +1081,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
@@ -1067,7 +1097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1090,7 +1120,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
@@ -1101,7 +1131,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
         <v>29</v>
@@ -1112,7 +1142,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
         <v>31</v>
@@ -1129,10 +1159,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1156,92 +1186,89 @@
       <c r="A2" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="1">
-        <v>626624.99</v>
-      </c>
-      <c r="C2" s="3">
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="2">
         <v>419522.88</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2487651.48</v>
-      </c>
-      <c r="C3" s="3">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="2">
         <v>1298604.49</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3580420.55</v>
-      </c>
-      <c r="C4" s="3">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="2">
         <v>1340324.3400000001</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="1">
-        <v>4883217.96</v>
-      </c>
-      <c r="C5" s="3">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="2">
         <v>1541061.48</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="1">
-        <v>5136589.43</v>
-      </c>
-      <c r="C6" s="3">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="2">
         <v>2141138.69</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="1">
-        <v>5076097.29</v>
-      </c>
-      <c r="C7" s="3">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="2">
         <v>1765909.85</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="1">
-        <v>6674722.0899999999</v>
-      </c>
-      <c r="C8" s="3">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="2">
         <v>1775147.16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="1">
-        <v>3395628.58</v>
-      </c>
-      <c r="C9" s="3">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="2">
         <v>963642.56</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="C10" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1266,21 +1293,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B2">
         <v>29833145.190000001</v>
@@ -1294,7 +1321,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B3">
         <v>2027807.18</v>
@@ -1329,10 +1356,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C1" t="s">
         <v>34</v>
@@ -1340,9 +1367,9 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" s="2">
+        <v>62</v>
+      </c>
+      <c r="B2" s="3">
         <v>0</v>
       </c>
       <c r="C2">
@@ -1351,9 +1378,9 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="2">
+        <v>63</v>
+      </c>
+      <c r="B3" s="3">
         <v>0</v>
       </c>
       <c r="C3">
@@ -1362,9 +1389,9 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="2">
+        <v>62</v>
+      </c>
+      <c r="B4" s="3">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="C4">
@@ -1373,9 +1400,9 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="2">
+        <v>63</v>
+      </c>
+      <c r="B5" s="3">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="C5">
@@ -1384,9 +1411,9 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" s="2">
+        <v>62</v>
+      </c>
+      <c r="B6" s="3">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C6">
@@ -1395,9 +1422,9 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="2">
+        <v>63</v>
+      </c>
+      <c r="B7" s="3">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C7">
@@ -1406,9 +1433,9 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="2">
+        <v>62</v>
+      </c>
+      <c r="B8" s="3">
         <v>0.125</v>
       </c>
       <c r="C8">
@@ -1417,9 +1444,9 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="2">
+        <v>63</v>
+      </c>
+      <c r="B9" s="3">
         <v>0.125</v>
       </c>
       <c r="C9">
@@ -1428,9 +1455,9 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="2">
+        <v>62</v>
+      </c>
+      <c r="B10" s="3">
         <v>0.16666666666666666</v>
       </c>
       <c r="C10">
@@ -1439,9 +1466,9 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" s="2">
+        <v>63</v>
+      </c>
+      <c r="B11" s="3">
         <v>0.16666666666666666</v>
       </c>
       <c r="C11">
@@ -1450,9 +1477,9 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12" s="2">
+        <v>62</v>
+      </c>
+      <c r="B12" s="3">
         <v>0.20833333333333334</v>
       </c>
       <c r="C12">
@@ -1461,9 +1488,9 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B13" s="2">
+        <v>63</v>
+      </c>
+      <c r="B13" s="3">
         <v>0.20833333333333334</v>
       </c>
       <c r="C13">
@@ -1472,9 +1499,9 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" s="2">
+        <v>62</v>
+      </c>
+      <c r="B14" s="3">
         <v>0.25</v>
       </c>
       <c r="C14">
@@ -1483,9 +1510,9 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" s="2">
+        <v>63</v>
+      </c>
+      <c r="B15" s="3">
         <v>0.25</v>
       </c>
       <c r="C15">
@@ -1494,9 +1521,9 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" s="2">
+        <v>62</v>
+      </c>
+      <c r="B16" s="3">
         <v>0.29166666666666669</v>
       </c>
       <c r="C16">
@@ -1505,9 +1532,9 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" s="2">
+        <v>63</v>
+      </c>
+      <c r="B17" s="3">
         <v>0.29166666666666669</v>
       </c>
       <c r="C17">
@@ -1516,9 +1543,9 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="2">
+        <v>62</v>
+      </c>
+      <c r="B18" s="3">
         <v>0.33333333333333331</v>
       </c>
       <c r="C18">
@@ -1527,9 +1554,9 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" s="2">
+        <v>63</v>
+      </c>
+      <c r="B19" s="3">
         <v>0.33333333333333331</v>
       </c>
       <c r="C19">
@@ -1538,9 +1565,9 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>54</v>
-      </c>
-      <c r="B20" s="2">
+        <v>62</v>
+      </c>
+      <c r="B20" s="3">
         <v>0.375</v>
       </c>
       <c r="C20">
@@ -1549,9 +1576,9 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" s="2">
+        <v>63</v>
+      </c>
+      <c r="B21" s="3">
         <v>0.375</v>
       </c>
       <c r="C21">
@@ -1560,9 +1587,9 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="2">
+        <v>62</v>
+      </c>
+      <c r="B22" s="3">
         <v>0.41666666666666669</v>
       </c>
       <c r="C22">
@@ -1571,9 +1598,9 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" s="2">
+        <v>63</v>
+      </c>
+      <c r="B23" s="3">
         <v>0.41666666666666669</v>
       </c>
       <c r="C23">
@@ -1582,9 +1609,9 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="2">
+        <v>62</v>
+      </c>
+      <c r="B24" s="3">
         <v>0.45833333333333331</v>
       </c>
       <c r="C24">
@@ -1593,9 +1620,9 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" s="2">
+        <v>63</v>
+      </c>
+      <c r="B25" s="3">
         <v>0.45833333333333331</v>
       </c>
       <c r="C25">
@@ -1604,9 +1631,9 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="2">
+        <v>62</v>
+      </c>
+      <c r="B26" s="3">
         <v>0.5</v>
       </c>
       <c r="C26">
@@ -1615,9 +1642,9 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>55</v>
-      </c>
-      <c r="B27" s="2">
+        <v>63</v>
+      </c>
+      <c r="B27" s="3">
         <v>0.5</v>
       </c>
       <c r="C27">
@@ -1626,9 +1653,9 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28" s="2">
+        <v>62</v>
+      </c>
+      <c r="B28" s="3">
         <v>0.54166666666666663</v>
       </c>
       <c r="C28">
@@ -1637,9 +1664,9 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" s="2">
+        <v>63</v>
+      </c>
+      <c r="B29" s="3">
         <v>0.54166666666666663</v>
       </c>
       <c r="C29">
@@ -1648,9 +1675,9 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="2">
+        <v>62</v>
+      </c>
+      <c r="B30" s="3">
         <v>0.58333333333333337</v>
       </c>
       <c r="C30">
@@ -1659,9 +1686,9 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>55</v>
-      </c>
-      <c r="B31" s="2">
+        <v>63</v>
+      </c>
+      <c r="B31" s="3">
         <v>0.58333333333333337</v>
       </c>
       <c r="C31">
@@ -1670,9 +1697,9 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" s="2">
+        <v>62</v>
+      </c>
+      <c r="B32" s="3">
         <v>0.625</v>
       </c>
       <c r="C32">
@@ -1681,9 +1708,9 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>55</v>
-      </c>
-      <c r="B33" s="2">
+        <v>63</v>
+      </c>
+      <c r="B33" s="3">
         <v>0.625</v>
       </c>
       <c r="C33">
@@ -1692,9 +1719,9 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>54</v>
-      </c>
-      <c r="B34" s="2">
+        <v>62</v>
+      </c>
+      <c r="B34" s="3">
         <v>0.66666666666666663</v>
       </c>
       <c r="C34">
@@ -1703,9 +1730,9 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>55</v>
-      </c>
-      <c r="B35" s="2">
+        <v>63</v>
+      </c>
+      <c r="B35" s="3">
         <v>0.66666666666666663</v>
       </c>
       <c r="C35">
@@ -1714,9 +1741,9 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>54</v>
-      </c>
-      <c r="B36" s="2">
+        <v>62</v>
+      </c>
+      <c r="B36" s="3">
         <v>0.70833333333333337</v>
       </c>
       <c r="C36">
@@ -1725,9 +1752,9 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>55</v>
-      </c>
-      <c r="B37" s="2">
+        <v>63</v>
+      </c>
+      <c r="B37" s="3">
         <v>0.70833333333333337</v>
       </c>
       <c r="C37">
@@ -1736,9 +1763,9 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>54</v>
-      </c>
-      <c r="B38" s="2">
+        <v>62</v>
+      </c>
+      <c r="B38" s="3">
         <v>0.75</v>
       </c>
       <c r="C38">
@@ -1747,9 +1774,9 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>55</v>
-      </c>
-      <c r="B39" s="2">
+        <v>63</v>
+      </c>
+      <c r="B39" s="3">
         <v>0.75</v>
       </c>
       <c r="C39">
@@ -1758,9 +1785,9 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>54</v>
-      </c>
-      <c r="B40" s="2">
+        <v>62</v>
+      </c>
+      <c r="B40" s="3">
         <v>0.79166666666666663</v>
       </c>
       <c r="C40">
@@ -1769,9 +1796,9 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>55</v>
-      </c>
-      <c r="B41" s="2">
+        <v>63</v>
+      </c>
+      <c r="B41" s="3">
         <v>0.79166666666666663</v>
       </c>
       <c r="C41">
@@ -1780,9 +1807,9 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>54</v>
-      </c>
-      <c r="B42" s="2">
+        <v>62</v>
+      </c>
+      <c r="B42" s="3">
         <v>0.83333333333333337</v>
       </c>
       <c r="C42">
@@ -1791,9 +1818,9 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>55</v>
-      </c>
-      <c r="B43" s="2">
+        <v>63</v>
+      </c>
+      <c r="B43" s="3">
         <v>0.83333333333333337</v>
       </c>
       <c r="C43">
@@ -1802,9 +1829,9 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>54</v>
-      </c>
-      <c r="B44" s="2">
+        <v>62</v>
+      </c>
+      <c r="B44" s="3">
         <v>0.875</v>
       </c>
       <c r="C44">
@@ -1813,9 +1840,9 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>55</v>
-      </c>
-      <c r="B45" s="2">
+        <v>63</v>
+      </c>
+      <c r="B45" s="3">
         <v>0.875</v>
       </c>
       <c r="C45">
@@ -1824,9 +1851,9 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>54</v>
-      </c>
-      <c r="B46" s="2">
+        <v>62</v>
+      </c>
+      <c r="B46" s="3">
         <v>0.91666666666666663</v>
       </c>
       <c r="C46">
@@ -1835,9 +1862,9 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>55</v>
-      </c>
-      <c r="B47" s="2">
+        <v>63</v>
+      </c>
+      <c r="B47" s="3">
         <v>0.91666666666666663</v>
       </c>
       <c r="C47">
@@ -1846,9 +1873,9 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>54</v>
-      </c>
-      <c r="B48" s="2">
+        <v>62</v>
+      </c>
+      <c r="B48" s="3">
         <v>0.95833333333333337</v>
       </c>
       <c r="C48">
@@ -1857,9 +1884,9 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>55</v>
-      </c>
-      <c r="B49" s="2">
+        <v>63</v>
+      </c>
+      <c r="B49" s="3">
         <v>0.95833333333333337</v>
       </c>
       <c r="C49">
@@ -1889,21 +1916,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B2">
         <v>28527002.210000001</v>
@@ -1917,7 +1944,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B3">
         <v>1626933.96</v>

</xml_diff>

<commit_message>
Auto commit at 2025-09-02 14:13:45.22
</commit_message>
<xml_diff>
--- a/data/cddata.xlsx
+++ b/data/cddata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
     <sheet name="Sheet10" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -196,10 +196,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3,395,628.58 kWh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2022年</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -363,6 +359,10 @@
   </si>
   <si>
     <t>华为</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3,919,250.91 kWh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -739,15 +739,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -755,7 +755,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -763,15 +763,15 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -779,7 +779,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -787,7 +787,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -795,7 +795,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
@@ -803,10 +803,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -820,7 +820,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -897,7 +897,7 @@
         <v>2025</v>
       </c>
       <c r="B9">
-        <v>3395628.58</v>
+        <v>3919250.9099999997</v>
       </c>
     </row>
   </sheetData>
@@ -910,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -930,7 +930,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -938,7 +938,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -946,7 +946,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -954,7 +954,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>14</v>
@@ -962,7 +962,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -998,7 +998,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
@@ -1006,7 +1006,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
@@ -1014,7 +1014,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -1022,7 +1022,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
@@ -1039,7 +1039,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1057,7 +1057,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
@@ -1065,7 +1065,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
         <v>21</v>
@@ -1073,7 +1073,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
@@ -1081,7 +1081,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
@@ -1097,14 +1097,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="13.125" customWidth="1"/>
-    <col min="2" max="2" width="22.25" customWidth="1"/>
+    <col min="2" max="3" width="22.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
@@ -1120,7 +1120,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
@@ -1131,7 +1131,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
         <v>29</v>
@@ -1142,7 +1142,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" t="s">
         <v>31</v>
@@ -1162,7 +1162,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1228,7 +1228,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
         <v>43</v>
@@ -1239,7 +1239,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
         <v>44</v>
@@ -1250,7 +1250,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
         <v>45</v>
@@ -1261,13 +1261,13 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="C9" s="2">
-        <v>963642.56</v>
+        <v>1129365.68</v>
       </c>
     </row>
   </sheetData>
@@ -1281,7 +1281,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1293,21 +1293,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>52</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>53</v>
-      </c>
-      <c r="D1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2">
         <v>29833145.190000001</v>
@@ -1321,7 +1321,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3">
         <v>2027807.18</v>
@@ -1356,10 +1356,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
         <v>34</v>
@@ -1367,7 +1367,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="3">
         <v>0</v>
@@ -1378,7 +1378,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="3">
         <v>0</v>
@@ -1389,7 +1389,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" s="3">
         <v>4.1666666666666664E-2</v>
@@ -1400,7 +1400,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="3">
         <v>4.1666666666666664E-2</v>
@@ -1411,7 +1411,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" s="3">
         <v>8.3333333333333329E-2</v>
@@ -1422,7 +1422,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7" s="3">
         <v>8.3333333333333329E-2</v>
@@ -1433,7 +1433,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="3">
         <v>0.125</v>
@@ -1444,7 +1444,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9" s="3">
         <v>0.125</v>
@@ -1455,7 +1455,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B10" s="3">
         <v>0.16666666666666666</v>
@@ -1466,7 +1466,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B11" s="3">
         <v>0.16666666666666666</v>
@@ -1477,7 +1477,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="3">
         <v>0.20833333333333334</v>
@@ -1488,7 +1488,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" s="3">
         <v>0.20833333333333334</v>
@@ -1499,7 +1499,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" s="3">
         <v>0.25</v>
@@ -1510,7 +1510,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15" s="3">
         <v>0.25</v>
@@ -1521,7 +1521,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B16" s="3">
         <v>0.29166666666666669</v>
@@ -1532,7 +1532,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B17" s="3">
         <v>0.29166666666666669</v>
@@ -1543,7 +1543,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18" s="3">
         <v>0.33333333333333331</v>
@@ -1554,7 +1554,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B19" s="3">
         <v>0.33333333333333331</v>
@@ -1565,7 +1565,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B20" s="3">
         <v>0.375</v>
@@ -1576,7 +1576,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B21" s="3">
         <v>0.375</v>
@@ -1587,7 +1587,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B22" s="3">
         <v>0.41666666666666669</v>
@@ -1598,7 +1598,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B23" s="3">
         <v>0.41666666666666669</v>
@@ -1609,7 +1609,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B24" s="3">
         <v>0.45833333333333331</v>
@@ -1620,7 +1620,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B25" s="3">
         <v>0.45833333333333331</v>
@@ -1631,7 +1631,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B26" s="3">
         <v>0.5</v>
@@ -1642,7 +1642,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B27" s="3">
         <v>0.5</v>
@@ -1653,7 +1653,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28" s="3">
         <v>0.54166666666666663</v>
@@ -1664,7 +1664,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B29" s="3">
         <v>0.54166666666666663</v>
@@ -1675,7 +1675,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B30" s="3">
         <v>0.58333333333333337</v>
@@ -1686,7 +1686,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B31" s="3">
         <v>0.58333333333333337</v>
@@ -1697,7 +1697,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B32" s="3">
         <v>0.625</v>
@@ -1708,7 +1708,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B33" s="3">
         <v>0.625</v>
@@ -1719,7 +1719,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B34" s="3">
         <v>0.66666666666666663</v>
@@ -1730,7 +1730,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B35" s="3">
         <v>0.66666666666666663</v>
@@ -1741,7 +1741,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B36" s="3">
         <v>0.70833333333333337</v>
@@ -1752,7 +1752,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B37" s="3">
         <v>0.70833333333333337</v>
@@ -1763,7 +1763,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B38" s="3">
         <v>0.75</v>
@@ -1774,7 +1774,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B39" s="3">
         <v>0.75</v>
@@ -1785,7 +1785,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B40" s="3">
         <v>0.79166666666666663</v>
@@ -1796,7 +1796,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B41" s="3">
         <v>0.79166666666666663</v>
@@ -1807,7 +1807,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B42" s="3">
         <v>0.83333333333333337</v>
@@ -1818,7 +1818,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B43" s="3">
         <v>0.83333333333333337</v>
@@ -1829,7 +1829,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B44" s="3">
         <v>0.875</v>
@@ -1840,7 +1840,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B45" s="3">
         <v>0.875</v>
@@ -1851,7 +1851,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B46" s="3">
         <v>0.91666666666666663</v>
@@ -1862,7 +1862,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B47" s="3">
         <v>0.91666666666666663</v>
@@ -1873,7 +1873,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B48" s="3">
         <v>0.95833333333333337</v>
@@ -1884,7 +1884,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B49" s="3">
         <v>0.95833333333333337</v>
@@ -1916,21 +1916,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
         <v>56</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>57</v>
-      </c>
-      <c r="D1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2">
         <v>28527002.210000001</v>
@@ -1944,7 +1944,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3">
         <v>1626933.96</v>

</xml_diff>

<commit_message>
Auto commit at 2025-09-03  9:35:54.86
</commit_message>
<xml_diff>
--- a/data/cddata.xlsx
+++ b/data/cddata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,57 +67,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>31,860,952.37kwh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>945,926.88 小时</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>30,153,936.17 元</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11,245,351.44 元</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1,228,315 笔</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>29,833,145.19 kwh</t>
-  </si>
-  <si>
-    <t>896,373.63 小时</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10,836,395.49 元</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1,157,944 笔</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2,027,807.18 kwh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>49,553.25 小时</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>408,955.96 元</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>70,371 笔</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>设备名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -136,18 +85,6 @@
     <t>¥1,622,108.79元</t>
   </si>
   <si>
-    <t>26,553,308.5kwh</t>
-  </si>
-  <si>
-    <t>¥9,214,286.69元</t>
-  </si>
-  <si>
-    <t>2,027,807.18kwh</t>
-  </si>
-  <si>
-    <t>¥408,955.96元</t>
-  </si>
-  <si>
     <t>年份</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -363,6 +300,74 @@
   </si>
   <si>
     <t>3,919,250.91 kWh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>32,415,190.21kwh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>959,954.47 小时</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30,602,748.99 元</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11,411,074.56 元</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,248,787 笔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30,203,491.59 kwh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>906,893.44小时</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10,963,759.73 元</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,173,045 笔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2,181,083.12kwh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>53,061.03 小时</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>447,314.84 元</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>75,742 笔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>26,960,145.05kwh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>¥9,350,570.29元</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>116,785.79kwh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>¥438,395.48元</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -370,8 +375,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;¥&quot;#,##0.00;[Red]&quot;¥&quot;\-#,##0.00"/>
+    <numFmt numFmtId="180" formatCode="#,##0.00_ "/>
+    <numFmt numFmtId="181" formatCode="#,##0.0_ "/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -409,11 +416,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -739,15 +749,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -755,7 +765,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -763,15 +773,15 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -779,7 +789,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -787,7 +797,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -795,7 +805,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
@@ -803,10 +813,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -830,10 +840,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
@@ -908,19 +918,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="2" max="2" width="22.375" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="15.625" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -928,45 +941,54 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+        <v>73</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+        <v>74</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+        <v>75</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="E6" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -976,19 +998,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15.875" customWidth="1"/>
     <col min="2" max="2" width="18.75" customWidth="1"/>
+    <col min="3" max="3" width="17.375" customWidth="1"/>
+    <col min="4" max="4" width="15.875" customWidth="1"/>
+    <col min="5" max="5" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -996,37 +1021,45 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+        <v>77</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+        <v>78</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+        <v>79</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="E5" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1036,18 +1069,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="2" width="23.125" customWidth="1"/>
+    <col min="3" max="3" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.375" customWidth="1"/>
+    <col min="5" max="5" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1055,37 +1091,45 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+        <v>82</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+        <v>83</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="E5" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1095,61 +1139,72 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="13.125" customWidth="1"/>
     <col min="2" max="3" width="22.25" customWidth="1"/>
+    <col min="4" max="4" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
         <v>85</v>
       </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>86</v>
       </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D3" s="5"/>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
         <v>87</v>
       </c>
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
       <c r="C4" t="s">
-        <v>32</v>
-      </c>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="C8" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1173,21 +1228,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2">
         <v>419522.88</v>
@@ -1195,10 +1250,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="C3" s="2">
         <v>1298604.49</v>
@@ -1206,10 +1261,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2">
         <v>1340324.3400000001</v>
@@ -1217,10 +1272,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C5" s="2">
         <v>1541061.48</v>
@@ -1228,10 +1283,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2">
         <v>2141138.69</v>
@@ -1239,10 +1294,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2">
         <v>1765909.85</v>
@@ -1250,10 +1305,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C8" s="2">
         <v>1775147.16</v>
@@ -1261,10 +1316,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="C9" s="2">
         <v>1129365.68</v>
@@ -1278,60 +1333,66 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="13.75" customWidth="1"/>
+    <col min="2" max="2" width="16.125" customWidth="1"/>
     <col min="3" max="3" width="17.625" customWidth="1"/>
     <col min="4" max="4" width="18.375" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2">
-        <v>29833145.190000001</v>
-      </c>
-      <c r="C2">
-        <v>10836395.49</v>
+        <v>42</v>
+      </c>
+      <c r="B2" s="5">
+        <v>30203491.59</v>
+      </c>
+      <c r="C2" s="5">
+        <v>10963759.73</v>
       </c>
       <c r="D2">
-        <v>1157944</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+        <v>1173045</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3">
-        <v>2027807.18</v>
-      </c>
-      <c r="C3">
-        <v>408955.96</v>
+        <v>43</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2181083.12</v>
+      </c>
+      <c r="C3" s="5">
+        <v>447314.84</v>
       </c>
       <c r="D3">
-        <v>70371</v>
-      </c>
+        <v>72742</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1356,18 +1417,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3">
         <v>0</v>
@@ -1378,7 +1439,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B3" s="3">
         <v>0</v>
@@ -1389,7 +1450,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B4" s="3">
         <v>4.1666666666666664E-2</v>
@@ -1400,7 +1461,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B5" s="3">
         <v>4.1666666666666664E-2</v>
@@ -1411,7 +1472,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B6" s="3">
         <v>8.3333333333333329E-2</v>
@@ -1422,7 +1483,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B7" s="3">
         <v>8.3333333333333329E-2</v>
@@ -1433,7 +1494,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B8" s="3">
         <v>0.125</v>
@@ -1444,7 +1505,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B9" s="3">
         <v>0.125</v>
@@ -1455,7 +1516,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B10" s="3">
         <v>0.16666666666666666</v>
@@ -1466,7 +1527,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B11" s="3">
         <v>0.16666666666666666</v>
@@ -1477,7 +1538,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B12" s="3">
         <v>0.20833333333333334</v>
@@ -1488,7 +1549,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B13" s="3">
         <v>0.20833333333333334</v>
@@ -1499,7 +1560,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B14" s="3">
         <v>0.25</v>
@@ -1510,7 +1571,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B15" s="3">
         <v>0.25</v>
@@ -1521,7 +1582,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B16" s="3">
         <v>0.29166666666666669</v>
@@ -1532,7 +1593,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B17" s="3">
         <v>0.29166666666666669</v>
@@ -1543,7 +1604,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B18" s="3">
         <v>0.33333333333333331</v>
@@ -1554,7 +1615,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B19" s="3">
         <v>0.33333333333333331</v>
@@ -1565,7 +1626,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B20" s="3">
         <v>0.375</v>
@@ -1576,7 +1637,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B21" s="3">
         <v>0.375</v>
@@ -1587,7 +1648,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B22" s="3">
         <v>0.41666666666666669</v>
@@ -1598,7 +1659,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B23" s="3">
         <v>0.41666666666666669</v>
@@ -1609,7 +1670,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B24" s="3">
         <v>0.45833333333333331</v>
@@ -1620,7 +1681,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B25" s="3">
         <v>0.45833333333333331</v>
@@ -1631,7 +1692,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B26" s="3">
         <v>0.5</v>
@@ -1642,7 +1703,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B27" s="3">
         <v>0.5</v>
@@ -1653,7 +1714,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B28" s="3">
         <v>0.54166666666666663</v>
@@ -1664,7 +1725,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B29" s="3">
         <v>0.54166666666666663</v>
@@ -1675,7 +1736,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B30" s="3">
         <v>0.58333333333333337</v>
@@ -1686,7 +1747,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B31" s="3">
         <v>0.58333333333333337</v>
@@ -1697,7 +1758,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B32" s="3">
         <v>0.625</v>
@@ -1708,7 +1769,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B33" s="3">
         <v>0.625</v>
@@ -1719,7 +1780,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B34" s="3">
         <v>0.66666666666666663</v>
@@ -1730,7 +1791,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B35" s="3">
         <v>0.66666666666666663</v>
@@ -1741,7 +1802,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B36" s="3">
         <v>0.70833333333333337</v>
@@ -1752,7 +1813,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B37" s="3">
         <v>0.70833333333333337</v>
@@ -1763,7 +1824,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B38" s="3">
         <v>0.75</v>
@@ -1774,7 +1835,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B39" s="3">
         <v>0.75</v>
@@ -1785,7 +1846,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B40" s="3">
         <v>0.79166666666666663</v>
@@ -1796,7 +1857,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B41" s="3">
         <v>0.79166666666666663</v>
@@ -1807,7 +1868,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B42" s="3">
         <v>0.83333333333333337</v>
@@ -1818,7 +1879,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B43" s="3">
         <v>0.83333333333333337</v>
@@ -1829,7 +1890,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B44" s="3">
         <v>0.875</v>
@@ -1840,7 +1901,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B45" s="3">
         <v>0.875</v>
@@ -1851,7 +1912,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B46" s="3">
         <v>0.91666666666666663</v>
@@ -1862,7 +1923,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B47" s="3">
         <v>0.91666666666666663</v>
@@ -1873,7 +1934,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B48" s="3">
         <v>0.95833333333333337</v>
@@ -1884,7 +1945,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B49" s="3">
         <v>0.95833333333333337</v>
@@ -1901,10 +1962,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1912,49 +1973,55 @@
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="16.375" customWidth="1"/>
     <col min="4" max="4" width="17.875" customWidth="1"/>
+    <col min="6" max="6" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2">
-        <v>28527002.210000001</v>
-      </c>
-      <c r="C2">
-        <v>17690606.73</v>
-      </c>
-      <c r="D2">
-        <v>10836395.48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+        <v>42</v>
+      </c>
+      <c r="B2" s="5">
+        <v>28846951.32</v>
+      </c>
+      <c r="C2" s="6">
+        <v>17883191.600000001</v>
+      </c>
+      <c r="D2" s="5">
+        <v>10963759.719999999</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3">
-        <v>1626933.96</v>
-      </c>
-      <c r="C3">
-        <v>1217978</v>
-      </c>
-      <c r="D3">
-        <v>408955.96</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1755797.67</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1308482.83</v>
+      </c>
+      <c r="D3" s="5">
+        <v>447314.83999999985</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Auto commit at 2025-10-01 11:25:27.09
</commit_message>
<xml_diff>
--- a/data/cddata.xlsx
+++ b/data/cddata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -377,8 +377,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;¥&quot;#,##0.00;[Red]&quot;¥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="180" formatCode="#,##0.00_ "/>
-    <numFmt numFmtId="181" formatCode="#,##0.0_ "/>
+    <numFmt numFmtId="176" formatCode="#,##0.00_ "/>
+    <numFmt numFmtId="177" formatCode="#,##0.0_ "/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -422,8 +422,8 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -920,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1964,8 +1964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Auto commit at 2025-10-01 16:59:35.04
</commit_message>
<xml_diff>
--- a/data/cddata.xlsx
+++ b/data/cddata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,10 +37,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>142支</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2160kw</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -181,10 +177,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>15支</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>sfp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -368,6 +360,14 @@
   </si>
   <si>
     <t>¥438,395.48元</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16支</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>141支</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -730,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -741,23 +741,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -765,7 +765,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -773,15 +773,15 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -789,34 +789,34 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -840,10 +840,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
@@ -920,7 +920,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -935,26 +935,26 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -962,30 +962,30 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C4" s="1"/>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C5" s="1"/>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C6" s="4"/>
       <c r="E6" s="5"/>
@@ -1015,48 +1015,48 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C2" s="1"/>
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C3" s="1"/>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C4" s="1"/>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C5" s="4"/>
       <c r="E5" s="5"/>
@@ -1085,48 +1085,48 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C2" s="1"/>
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C3" s="1"/>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C4" s="1"/>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C5" s="4"/>
       <c r="E5" s="5"/>
@@ -1155,48 +1155,48 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
@@ -1228,21 +1228,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
         <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
       </c>
       <c r="C2" s="2">
         <v>419522.88</v>
@@ -1250,10 +1250,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
         <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
       </c>
       <c r="C3" s="2">
         <v>1298604.49</v>
@@ -1261,10 +1261,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="2">
         <v>1340324.3400000001</v>
@@ -1272,10 +1272,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2">
         <v>1541061.48</v>
@@ -1283,10 +1283,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2">
         <v>2141138.69</v>
@@ -1294,10 +1294,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="2">
         <v>1765909.85</v>
@@ -1305,10 +1305,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="2">
         <v>1775147.16</v>
@@ -1316,10 +1316,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C9" s="2">
         <v>1129365.68</v>
@@ -1350,21 +1350,21 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>35</v>
-      </c>
-      <c r="D1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2" s="5">
         <v>30203491.59</v>
@@ -1380,7 +1380,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B3" s="5">
         <v>2181083.12</v>
@@ -1417,18 +1417,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" s="3">
         <v>0</v>
@@ -1439,7 +1439,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B3" s="3">
         <v>0</v>
@@ -1450,7 +1450,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" s="3">
         <v>4.1666666666666664E-2</v>
@@ -1461,7 +1461,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B5" s="3">
         <v>4.1666666666666664E-2</v>
@@ -1472,7 +1472,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B6" s="3">
         <v>8.3333333333333329E-2</v>
@@ -1483,7 +1483,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B7" s="3">
         <v>8.3333333333333329E-2</v>
@@ -1494,7 +1494,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B8" s="3">
         <v>0.125</v>
@@ -1505,7 +1505,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9" s="3">
         <v>0.125</v>
@@ -1516,7 +1516,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B10" s="3">
         <v>0.16666666666666666</v>
@@ -1527,7 +1527,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B11" s="3">
         <v>0.16666666666666666</v>
@@ -1538,7 +1538,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B12" s="3">
         <v>0.20833333333333334</v>
@@ -1549,7 +1549,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B13" s="3">
         <v>0.20833333333333334</v>
@@ -1560,7 +1560,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B14" s="3">
         <v>0.25</v>
@@ -1571,7 +1571,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B15" s="3">
         <v>0.25</v>
@@ -1582,7 +1582,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B16" s="3">
         <v>0.29166666666666669</v>
@@ -1593,7 +1593,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B17" s="3">
         <v>0.29166666666666669</v>
@@ -1604,7 +1604,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B18" s="3">
         <v>0.33333333333333331</v>
@@ -1615,7 +1615,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B19" s="3">
         <v>0.33333333333333331</v>
@@ -1626,7 +1626,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B20" s="3">
         <v>0.375</v>
@@ -1637,7 +1637,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B21" s="3">
         <v>0.375</v>
@@ -1648,7 +1648,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B22" s="3">
         <v>0.41666666666666669</v>
@@ -1659,7 +1659,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B23" s="3">
         <v>0.41666666666666669</v>
@@ -1670,7 +1670,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B24" s="3">
         <v>0.45833333333333331</v>
@@ -1681,7 +1681,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B25" s="3">
         <v>0.45833333333333331</v>
@@ -1692,7 +1692,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B26" s="3">
         <v>0.5</v>
@@ -1703,7 +1703,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B27" s="3">
         <v>0.5</v>
@@ -1714,7 +1714,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B28" s="3">
         <v>0.54166666666666663</v>
@@ -1725,7 +1725,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B29" s="3">
         <v>0.54166666666666663</v>
@@ -1736,7 +1736,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B30" s="3">
         <v>0.58333333333333337</v>
@@ -1747,7 +1747,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B31" s="3">
         <v>0.58333333333333337</v>
@@ -1758,7 +1758,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B32" s="3">
         <v>0.625</v>
@@ -1769,7 +1769,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B33" s="3">
         <v>0.625</v>
@@ -1780,7 +1780,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B34" s="3">
         <v>0.66666666666666663</v>
@@ -1791,7 +1791,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B35" s="3">
         <v>0.66666666666666663</v>
@@ -1802,7 +1802,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B36" s="3">
         <v>0.70833333333333337</v>
@@ -1813,7 +1813,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B37" s="3">
         <v>0.70833333333333337</v>
@@ -1824,7 +1824,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B38" s="3">
         <v>0.75</v>
@@ -1835,7 +1835,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B39" s="3">
         <v>0.75</v>
@@ -1846,7 +1846,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B40" s="3">
         <v>0.79166666666666663</v>
@@ -1857,7 +1857,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B41" s="3">
         <v>0.79166666666666663</v>
@@ -1868,7 +1868,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B42" s="3">
         <v>0.83333333333333337</v>
@@ -1879,7 +1879,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B43" s="3">
         <v>0.83333333333333337</v>
@@ -1890,7 +1890,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B44" s="3">
         <v>0.875</v>
@@ -1901,7 +1901,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B45" s="3">
         <v>0.875</v>
@@ -1912,7 +1912,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B46" s="3">
         <v>0.91666666666666663</v>
@@ -1923,7 +1923,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B47" s="3">
         <v>0.91666666666666663</v>
@@ -1934,7 +1934,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B48" s="3">
         <v>0.95833333333333337</v>
@@ -1945,7 +1945,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B49" s="3">
         <v>0.95833333333333337</v>
@@ -1979,21 +1979,21 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>39</v>
-      </c>
-      <c r="D1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2" s="5">
         <v>28846951.32</v>
@@ -2009,7 +2009,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B3" s="5">
         <v>1755797.67</v>

</xml_diff>

<commit_message>
Auto commit at 2025-10-01 17:13:27.51
</commit_message>
<xml_diff>
--- a/data/cddata.xlsx
+++ b/data/cddata.xlsx
@@ -363,11 +363,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>142支</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>16支</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>141支</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -731,7 +731,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -776,7 +776,7 @@
         <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
@@ -808,7 +808,7 @@
         <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
@@ -816,7 +816,7 @@
         <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto commit at 2025-10-06  9:50:52.08
</commit_message>
<xml_diff>
--- a/data/cddata.xlsx
+++ b/data/cddata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -295,42 +295,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>32,415,190.21kwh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>959,954.47 小时</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>30,602,748.99 元</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11,411,074.56 元</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1,248,787 笔</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>30,203,491.59 kwh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>906,893.44小时</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10,963,759.73 元</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1,173,045 笔</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2,181,083.12kwh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -369,6 +337,34 @@
   <si>
     <t>16支</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>32,832,455.27kwh</t>
+  </si>
+  <si>
+    <t>32,832,455.27kwh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30,965,040.19 元</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11,552,311.03 元</t>
+  </si>
+  <si>
+    <t>11,552,311.03 元</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,266,628 笔</t>
+  </si>
+  <si>
+    <t>1,266,628 笔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>959,954.47 小时</t>
   </si>
 </sst>
 </file>
@@ -730,7 +726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -776,7 +772,7 @@
         <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
@@ -808,7 +804,7 @@
         <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
@@ -816,7 +812,7 @@
         <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -829,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -921,7 +917,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B5" sqref="B5:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -946,7 +942,7 @@
         <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -954,7 +950,7 @@
         <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -965,7 +961,7 @@
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="C4" s="1"/>
       <c r="E4" s="5"/>
@@ -975,7 +971,7 @@
         <v>55</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="C5" s="1"/>
       <c r="E5" s="5"/>
@@ -985,7 +981,7 @@
         <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="C6" s="4"/>
       <c r="E6" s="5"/>
@@ -1001,7 +997,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1026,7 +1022,7 @@
         <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C2" s="1"/>
       <c r="E2" s="5"/>
@@ -1036,7 +1032,7 @@
         <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="C3" s="1"/>
       <c r="E3" s="5"/>
@@ -1046,7 +1042,7 @@
         <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C4" s="1"/>
       <c r="E4" s="5"/>
@@ -1056,7 +1052,7 @@
         <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="C5" s="4"/>
       <c r="E5" s="5"/>
@@ -1096,7 +1092,7 @@
         <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C2" s="1"/>
       <c r="E2" s="5"/>
@@ -1106,7 +1102,7 @@
         <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C3" s="1"/>
       <c r="E3" s="5"/>
@@ -1116,7 +1112,7 @@
         <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C4" s="1"/>
       <c r="E4" s="5"/>
@@ -1126,7 +1122,7 @@
         <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C5" s="4"/>
       <c r="E5" s="5"/>
@@ -1142,7 +1138,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1180,10 +1176,10 @@
         <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="6"/>
@@ -1193,10 +1189,10 @@
         <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C4" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
@@ -1404,7 +1400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Auto commit at 2025-12-01 15:41:28.88
</commit_message>
<xml_diff>
--- a/data/cddata.xlsx
+++ b/data/cddata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -295,10 +295,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>959,954.47 小时</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2,181,083.12kwh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -339,32 +335,36 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>32,832,455.27kwh</t>
-  </si>
-  <si>
-    <t>32,832,455.27kwh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>30,965,040.19 元</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11,552,311.03 元</t>
-  </si>
-  <si>
-    <t>11,552,311.03 元</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1,266,628 笔</t>
-  </si>
-  <si>
-    <t>1,266,628 笔</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>959,954.47 小时</t>
+    <t>33,668,088.1kwh</t>
+  </si>
+  <si>
+    <t>33,668,088.1kwh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>31,675,628.12 元</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11,813,678.92 元</t>
+  </si>
+  <si>
+    <t>11,813,678.92 元</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,300,337 笔</t>
+  </si>
+  <si>
+    <t>1,300,337 笔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>995,921.95 小时</t>
+  </si>
+  <si>
+    <t>995,921.95 小时</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -772,7 +772,7 @@
         <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
@@ -804,7 +804,7 @@
         <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
@@ -812,7 +812,7 @@
         <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -825,13 +825,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="21.625" customWidth="1"/>
+    <col min="5" max="5" width="18.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
@@ -871,7 +872,7 @@
         <v>2021</v>
       </c>
       <c r="B5">
-        <v>4883217.96</v>
+        <v>4883275.16</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
@@ -903,7 +904,7 @@
         <v>2025</v>
       </c>
       <c r="B9">
-        <v>3919250.9099999997</v>
+        <v>5202707.1199999992</v>
       </c>
     </row>
   </sheetData>
@@ -942,7 +943,7 @@
         <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -950,7 +951,7 @@
         <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -961,7 +962,7 @@
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4" s="1"/>
       <c r="E4" s="5"/>
@@ -971,7 +972,7 @@
         <v>55</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C5" s="1"/>
       <c r="E5" s="5"/>
@@ -981,7 +982,7 @@
         <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C6" s="4"/>
       <c r="E6" s="5"/>
@@ -997,7 +998,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1022,7 +1023,7 @@
         <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2" s="1"/>
       <c r="E2" s="5"/>
@@ -1032,7 +1033,7 @@
         <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C3" s="1"/>
       <c r="E3" s="5"/>
@@ -1042,7 +1043,7 @@
         <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" s="1"/>
       <c r="E4" s="5"/>
@@ -1052,7 +1053,7 @@
         <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C5" s="4"/>
       <c r="E5" s="5"/>
@@ -1067,7 +1068,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1092,7 +1093,7 @@
         <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
       <c r="E2" s="5"/>
@@ -1102,7 +1103,7 @@
         <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3" s="1"/>
       <c r="E3" s="5"/>
@@ -1112,7 +1113,7 @@
         <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4" s="1"/>
       <c r="E4" s="5"/>
@@ -1122,7 +1123,7 @@
         <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C5" s="4"/>
       <c r="E5" s="5"/>
@@ -1176,10 +1177,10 @@
         <v>67</v>
       </c>
       <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
         <v>75</v>
-      </c>
-      <c r="C3" t="s">
-        <v>76</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="6"/>
@@ -1189,10 +1190,10 @@
         <v>68</v>
       </c>
       <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="s">
         <v>77</v>
-      </c>
-      <c r="C4" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
@@ -1332,7 +1333,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1363,13 +1364,13 @@
         <v>40</v>
       </c>
       <c r="B2" s="5">
-        <v>30203491.59</v>
+        <v>31068378.629999999</v>
       </c>
       <c r="C2" s="5">
-        <v>10963759.73</v>
-      </c>
-      <c r="D2">
-        <v>1173045</v>
+        <v>11258877.66</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1209488</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -1379,13 +1380,13 @@
         <v>41</v>
       </c>
       <c r="B3" s="5">
-        <v>2181083.12</v>
+        <v>2599709.4700000002</v>
       </c>
       <c r="C3" s="5">
-        <v>447314.84</v>
+        <v>554801.26</v>
       </c>
       <c r="D3">
-        <v>72742</v>
+        <v>90849</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -1961,7 +1962,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1992,13 +1993,13 @@
         <v>40</v>
       </c>
       <c r="B2" s="5">
-        <v>28846951.32</v>
+        <v>29573852.800000001</v>
       </c>
       <c r="C2" s="6">
-        <v>17883191.600000001</v>
+        <v>18314975.129999999</v>
       </c>
       <c r="D2" s="5">
-        <v>10963759.719999999</v>
+        <v>11258877.66</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -2008,13 +2009,13 @@
         <v>41</v>
       </c>
       <c r="B3" s="5">
-        <v>1755797.67</v>
+        <v>2101775.3199999998</v>
       </c>
       <c r="C3" s="5">
-        <v>1308482.83</v>
+        <v>1546974.06</v>
       </c>
       <c r="D3" s="5">
-        <v>447314.83999999985</v>
+        <v>554801.26</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>

</xml_diff>

<commit_message>
Auto commit at 2026-01-16  8:01:08.07
</commit_message>
<xml_diff>
--- a/data/cddata.xlsx
+++ b/data/cddata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -331,10 +331,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>16支</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>33,668,088.1kwh</t>
   </si>
   <si>
@@ -364,6 +360,10 @@
   </si>
   <si>
     <t>995,921.95 小时</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1支</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -727,7 +727,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -772,7 +772,7 @@
         <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
@@ -812,7 +812,7 @@
         <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -825,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -918,7 +918,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B6"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -943,7 +943,7 @@
         <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -951,7 +951,7 @@
         <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -962,7 +962,7 @@
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" s="1"/>
       <c r="E4" s="5"/>
@@ -972,7 +972,7 @@
         <v>55</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C5" s="1"/>
       <c r="E5" s="5"/>
@@ -982,7 +982,7 @@
         <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C6" s="4"/>
       <c r="E6" s="5"/>
@@ -1023,7 +1023,7 @@
         <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C2" s="1"/>
       <c r="E2" s="5"/>
@@ -1033,7 +1033,7 @@
         <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C3" s="1"/>
       <c r="E3" s="5"/>
@@ -1043,7 +1043,7 @@
         <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4" s="1"/>
       <c r="E4" s="5"/>
@@ -1053,7 +1053,7 @@
         <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C5" s="4"/>
       <c r="E5" s="5"/>
@@ -1068,7 +1068,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>

</xml_diff>